<commit_message>
mise à jour du tableau source
</commit_message>
<xml_diff>
--- a/schema-donnees-IDIA.xlsx
+++ b/schema-donnees-IDIA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc/idia-latex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc/idia-latex/maquette-idia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402BC4FA-8F86-0F44-A5AF-96B22E2CEBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABD603B-92B9-6B41-8262-B96F0D54F5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17480" yWindow="-24080" windowWidth="39780" windowHeight="26740" activeTab="3" xr2:uid="{A0D72F4E-CE78-7B4E-A3D3-46CC3737DF83}"/>
+    <workbookView xWindow="-17640" yWindow="-27120" windowWidth="33380" windowHeight="27120" activeTab="3" xr2:uid="{A0D72F4E-CE78-7B4E-A3D3-46CC3737DF83}"/>
   </bookViews>
   <sheets>
     <sheet name="description UE" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="138">
   <si>
     <t>NomUE</t>
   </si>
@@ -565,9 +565,6 @@
     </r>
   </si>
   <si>
-    <t>L'élément constitutif Techniques de Devops permet d’explorer l’écosystème d’outils utilisés dans le développement d'un logiciel, en comprendre les principes et pouvoir les configurer. Ces outils visent à automatiser la production du système final à partir des différents artefacts produits (code source) ou utilisés, estimer ou garantir la qualité, permettre à différentes personnes de travailler simultanément sur le même artefact, documenter l'évolution des artefacts au cours du temps, etc.</t>
-  </si>
-  <si>
     <t>L’élément constitutif Conception de systèmes d’information introduit différents principes, outils et langages de modélisation tels que UML ou les diagrammes Entités-Associations, dont la traduction vers le modèle relationnel est très précisément étudiée. Une palette riche de diagrammes est présentée, pour proposer des points de vue complémentaires dans l’activité de modélisation de SI : état-transition, flux, séquences, etc.</t>
   </si>
   <si>
@@ -668,6 +665,21 @@
   </si>
   <si>
     <t>Cette matière vise à permettre aux apprentis de passer d’une position «d’étudiant» à une position de «professionnel», grâce à une réflexion sur leurs modes et méthodologies d’apprentissage; une identification des pratiques efficientes;un échange entre pairs; une mise en lien des deux lieux de formation que sont l’école et l’entreprise d’accueil.</t>
+  </si>
+  <si>
+    <t>Cette matière vise à apporter une réflexion rétrospective sur l'expérience interculturelle, via des restitutions et des échanges, faisant suite au séjour à l'étranger.</t>
+  </si>
+  <si>
+    <t>La matière vise à sensibiliser à la démarche de modélisation de problème (choix des variables, conséquences, choix du critère d'optimalité, multiplicité des critères, questions de consensus), discuter des caractéristiques des espaces de recherche puis à présenter des techniques d'exploration-optimisation dans ces espaces.</t>
+  </si>
+  <si>
+    <t>En s'appuyant sur la connaissance d'un ou deux langages informatiques, la matière aborde quelques points complémentaires relative à la qualité et à la construction : le preuve de programme, l'analyse statique, la gestion des dépendances, les bonnes pratiques sur le développement collaboratifs (prise de recul sur les usages de git)</t>
+  </si>
+  <si>
+    <t>En s'appuyant sur des connaissances de base en développement et construction de logiciel, la matière prolonge ces compétences en y ajoutant l'intégration continue, la conteneurisation et le déploiement dans le cloud.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette matière sensibilise à l'apport du parallélisme pour la performance de traitement sur des données. La mise en correspondance entre "l'architecture" des problèmes et celles des infrastructures est discutée, ainsi que l'écriture d'algorithmes mettant en oeuvre ces opérateurs à parallélisation de données. </t>
   </si>
 </sst>
 </file>
@@ -755,7 +767,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -780,6 +792,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1161,7 +1176,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1192,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1203,7 +1218,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1214,7 +1229,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1234,7 +1249,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1245,7 +1260,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1256,7 +1271,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1267,7 +1282,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1287,7 +1302,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1298,18 +1313,18 @@
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="7">
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1320,7 +1335,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1363,7 +1378,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -1371,7 +1386,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1379,7 +1394,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1387,7 +1402,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -1395,7 +1410,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>48</v>
@@ -1403,7 +1418,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>37</v>
@@ -1411,7 +1426,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>36</v>
@@ -1419,7 +1434,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>35</v>
@@ -1427,7 +1442,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>34</v>
@@ -1435,7 +1450,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>51</v>
@@ -1502,7 +1517,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1965,7 +1980,7 @@
         <v>45</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1973,31 +1988,31 @@
         <v>45</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2005,7 +2020,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2013,7 +2028,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2021,7 +2036,7 @@
         <v>47</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2029,7 +2044,7 @@
         <v>44</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2037,7 +2052,7 @@
         <v>44</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2045,7 +2060,7 @@
         <v>44</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2053,7 +2068,7 @@
         <v>44</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2061,7 +2076,7 @@
         <v>45</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2069,7 +2084,7 @@
         <v>45</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2081,13 +2096,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D02417-9CF9-8E4A-BC10-352069006729}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50" customWidth="1"/>
+    <col min="1" max="1" width="39.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="83.83203125" style="5" customWidth="1"/>
     <col min="3" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="6" width="16.5" customWidth="1"/>
@@ -2095,7 +2110,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -2120,8 +2135,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="135" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="150" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -2147,7 +2162,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2173,7 +2188,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -2199,7 +2214,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2225,7 +2240,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2251,7 +2266,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2277,7 +2292,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -2303,7 +2318,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -2329,7 +2344,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2355,7 +2370,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="12" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2373,11 +2388,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="12" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
@@ -2385,7 +2400,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="150" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="12" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2397,7 +2412,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="12" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -2407,7 +2422,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="12" t="s">
         <v>89</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -2425,11 +2440,11 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2441,11 +2456,11 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
@@ -2456,7 +2471,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="12" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -2464,7 +2479,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -2472,71 +2487,71 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="153" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
     <row r="28" spans="1:8" ht="170" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="10" t="s">
         <v>60</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -2544,7 +2559,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="10" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -2552,7 +2567,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -2560,7 +2575,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="10" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -2568,259 +2583,259 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="10" t="s">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A58" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="10" t="s">
+    <row r="59" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A59" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A60" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
+    <row r="61" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="B61" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
+      <c r="B62" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="B63" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
amélioration des descriptions de matières
</commit_message>
<xml_diff>
--- a/schema-donnees-IDIA.xlsx
+++ b/schema-donnees-IDIA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc/idia-latex/maquette-idia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABD603B-92B9-6B41-8262-B96F0D54F5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D1824A-764F-9842-9A5A-F89C37A38850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17640" yWindow="-27120" windowWidth="33380" windowHeight="27120" activeTab="3" xr2:uid="{A0D72F4E-CE78-7B4E-A3D3-46CC3737DF83}"/>
+    <workbookView xWindow="-17960" yWindow="-28300" windowWidth="35880" windowHeight="27120" activeTab="3" xr2:uid="{A0D72F4E-CE78-7B4E-A3D3-46CC3737DF83}"/>
   </bookViews>
   <sheets>
     <sheet name="description UE" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="141">
   <si>
     <t>NomUE</t>
   </si>
@@ -571,9 +571,6 @@
     <t>L'élément constitutif Statistiques et probabilités étudie les concepts de base de la théorie des probabilités et les distributions les plus courantes, pour permettre la modélisation et la résolution des problèmes réels ou théoriques. En complément, il introduit au raisonnement statistique et à la prise en compte de l'aléa en situation de décision et permet de s’initier aux étapes principales d'une démarche statistique (décrire, estimer, tester).</t>
   </si>
   <si>
-    <t>Evaluation et optimisation de requête, algorithmes de tri et de jointure. Indexation (structures de données) et transcription des requêtes aux bases de données en algorithmes efficaces. Organisation physique et performance.</t>
-  </si>
-  <si>
     <t>Cette manière approfondit le domaine des bases de données en s'intéressant aux transactions, c’est-à-dire à l'analyse des problèmes soulevés par l'accès potentiellement concurrents d'accès aux bases de données. Les mécanismes et solutions sont exposés en ayant recours au contrôle de concurrence, l'isolation, la sérialisabilité, les verrous.</t>
   </si>
   <si>
@@ -595,9 +592,6 @@
     <t>Cette matière valorise dans la maquette pédagogique l'activité réalisée en entreprise, chaque semestre, par les apprenti.e.s.</t>
   </si>
   <si>
-    <t>L'élément constitutif SQL avancé et entrepôts de données aborde la modélisation de bases de données multidimensionnelles, conçues pour héberger toutes les données d’une organisation en vue de leur exploitation dans des systèmes décisionnels. En outre, nous abordons les mécanismes complexes et néanmoins utiles du langage SQL, tels que les requêtes récursives ou les requêtes analytiques, la division relationnelle ou encore les requêtes imbriquées.</t>
-  </si>
-  <si>
     <t>Web semantique</t>
   </si>
   <si>
@@ -670,9 +664,6 @@
     <t>Cette matière vise à apporter une réflexion rétrospective sur l'expérience interculturelle, via des restitutions et des échanges, faisant suite au séjour à l'étranger.</t>
   </si>
   <si>
-    <t>La matière vise à sensibiliser à la démarche de modélisation de problème (choix des variables, conséquences, choix du critère d'optimalité, multiplicité des critères, questions de consensus), discuter des caractéristiques des espaces de recherche puis à présenter des techniques d'exploration-optimisation dans ces espaces.</t>
-  </si>
-  <si>
     <t>En s'appuyant sur la connaissance d'un ou deux langages informatiques, la matière aborde quelques points complémentaires relative à la qualité et à la construction : le preuve de programme, l'analyse statique, la gestion des dépendances, les bonnes pratiques sur le développement collaboratifs (prise de recul sur les usages de git)</t>
   </si>
   <si>
@@ -680,6 +671,24 @@
   </si>
   <si>
     <t xml:space="preserve">Cette matière sensibilise à l'apport du parallélisme pour la performance de traitement sur des données. La mise en correspondance entre "l'architecture" des problèmes et celles des infrastructures est discutée, ainsi que l'écriture d'algorithmes mettant en oeuvre ces opérateurs à parallélisation de données. </t>
+  </si>
+  <si>
+    <t>Evaluation et optimisation de requête, algorithmes de tri et de jointure. Indexation (structures de données) et transcription des requêtes aux bases de données en plan d'execution algorithmique efficaces. Organisation physique et performance.</t>
+  </si>
+  <si>
+    <t>L'élément constitutif SQL avancé et entrepôts de données aborde la modélisation de bases de données multidimensionnelles, dont les spécificités architecturales sont conçues pour rendre efficacement disponibles toutes les données d’une organisation en vue de leur exploitation dans des systèmes décisionnels. En outre, nous abordons les mécanismes complexes et néanmoins utiles du langage SQL, tels que les requêtes récursives ou les requêtes analytiques, la division relationnelle ou encore les requêtes imbriquées.</t>
+  </si>
+  <si>
+    <t>Cette matière prolonge l'étude des bases et entrepôts de données vers les outils et les enjeux de la business intelligence, illustré sur l'outil PowerBI. L'objectif est une illustration proche de scénarii professionnels d'une chaîne intégrée dans le cloud (Azure) et une discussion sur les métiers.  C'est enfin l'occasion de discuter les choix en visualisation de données en fonction des variables et des objectifs.</t>
+  </si>
+  <si>
+    <t>La matière introduit les outils théoriques pour l'analyse multivariée de données (analyse en composantes principales, multidimensional scaling) et clustering et les illustre par une série de travaux pratiques sur divers jeux de données.</t>
+  </si>
+  <si>
+    <t>La matière vise à sensibiliser à la démarche de modélisation de problème (choix des variables, conséquences, choix du critère d'optimalité, multiplicité des critères, questions de consensus), discuter des caractéristiques des espaces de recherche puis à présenter des techniques d'exploration-optimisation dans ces espaces, dont la programmation linéaire et les métaheuristiques.</t>
+  </si>
+  <si>
+    <t>Dans un premier temps, la matière prend l'angle de l'exploration de graphes de recherche, s'appuy ant sur des techniques algorithmiques et/ou heuristiques ()</t>
   </si>
 </sst>
 </file>
@@ -767,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -794,8 +803,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1176,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1207,7 +1222,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1218,7 +1233,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1229,7 +1244,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1249,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1260,7 +1275,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1271,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1282,7 +1297,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1302,7 +1317,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1313,18 +1328,18 @@
         <v>5</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B19" s="7">
         <v>5</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1335,7 +1350,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1378,7 +1393,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -1386,7 +1401,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1394,7 +1409,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1402,7 +1417,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
@@ -1410,7 +1425,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>48</v>
@@ -1418,7 +1433,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>37</v>
@@ -1426,7 +1441,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>36</v>
@@ -1434,7 +1449,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>35</v>
@@ -1442,7 +1457,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>34</v>
@@ -1450,7 +1465,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>51</v>
@@ -1517,7 +1532,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1980,7 +1995,7 @@
         <v>45</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1988,31 +2003,31 @@
         <v>45</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2020,7 +2035,7 @@
         <v>47</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2028,7 +2043,7 @@
         <v>47</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2036,7 +2051,7 @@
         <v>47</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2044,7 +2059,7 @@
         <v>44</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2052,7 +2067,7 @@
         <v>44</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +2075,7 @@
         <v>44</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2068,7 +2083,7 @@
         <v>44</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -2076,7 +2091,7 @@
         <v>45</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -2084,7 +2099,7 @@
         <v>45</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2097,12 +2112,12 @@
   <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.5" style="5" customWidth="1"/>
+    <col min="1" max="1" width="39.5" style="12" customWidth="1"/>
     <col min="2" max="2" width="83.83203125" style="5" customWidth="1"/>
     <col min="3" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="6" width="16.5" customWidth="1"/>
@@ -2110,7 +2125,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -2136,7 +2151,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="150" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -2162,7 +2177,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="150" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2188,7 +2203,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -2214,7 +2229,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -2240,7 +2255,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -2266,7 +2281,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -2292,7 +2307,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -2318,7 +2333,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -2344,7 +2359,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2370,7 +2385,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -2388,11 +2403,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1">
@@ -2400,7 +2415,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="150" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -2412,7 +2427,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -2422,7 +2437,7 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -2440,11 +2455,11 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="12" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2456,11 +2471,11 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1">
@@ -2471,7 +2486,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="9" t="s">
@@ -2479,7 +2494,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>83</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -2487,15 +2502,15 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>52</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="14" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2503,15 +2518,15 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -2519,39 +2534,39 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="26" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="14" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="170" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="170" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -2559,7 +2574,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="14" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -2567,7 +2582,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="14" t="s">
         <v>66</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -2575,7 +2590,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="85" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -2583,259 +2598,259 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="14" t="s">
         <v>63</v>
       </c>
       <c r="B33" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A38" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="10" t="s">
+    <row r="39" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A40" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A45" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="10" t="s">
+    <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A46" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="10" t="s">
+    <row r="47" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A49" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="B51" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+      <c r="B59" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B60" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A59" s="10" t="s">
+    <row r="61" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A60" s="10" t="s">
+      <c r="B61" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A61" s="10" t="s">
+      <c r="B62" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="10" t="s">
-        <v>124</v>
-      </c>
       <c r="B63" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>